<commit_message>
Sweet new dropdowns for various fields
</commit_message>
<xml_diff>
--- a/bulk_edit_template.xlsx
+++ b/bulk_edit_template.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Records to Create" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Records to Update" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Vocabularies" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="174">
   <si>
     <t xml:space="preserve">Required</t>
   </si>
@@ -29,7 +30,7 @@
     <t xml:space="preserve">Optional</t>
   </si>
   <si>
-    <t xml:space="preserve">Required (PR/DR only)	</t>
+    <t xml:space="preserve">Required (PR only) </t>
   </si>
   <si>
     <t xml:space="preserve">Required (ITM only)</t>
@@ -92,7 +93,7 @@
     <t xml:space="preserve">Significance</t>
   </si>
   <si>
-    <t xml:space="preserve">Inherit Significance?</t>
+    <t xml:space="preserve">Don't inherit Significance changes</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright Status</t>
@@ -104,7 +105,7 @@
     <t xml:space="preserve">Remarks</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional (PR/DR only) </t>
+    <t xml:space="preserve">Optional (PR only) </t>
   </si>
   <si>
     <t xml:space="preserve">Optional (PR only)</t>
@@ -114,6 +115,435 @@
   </si>
   <si>
     <t xml:space="preserve">Record QSA ID (ITM, PR, DR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Qualifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approximate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architectural or technical drawing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This may contain information or photographs which some people may find distressing or offensive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copyright_expired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chart (produced by machine)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARCBX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This may contain terms or images which Aboriginal and Torres Strait Islander people may find distressing or offensive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iconic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copyright_state_of_queensland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drafting Cloth (Linen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memory_of_the_world</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Film (roll)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Box - Microfiche Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Cartridge Tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Cassette Tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compact Disc (CD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Floppy Disk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Hard Disc Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Versatile Disc (DVD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Reel Tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital media - Floppy disc - 3 1/2"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Reel Tape -- 21 Track</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital media - Floppy disc - 5 1/4"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Reel Tape -- 7 Track</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital media - Floppy disc - 8"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Reel Tape -- 9 Track</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital media - LTO computer tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Video Tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital media - Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Video Tape -- Betamax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital media - PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Video Tape -- U-Matic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital media - Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic Media -- Video Tape -- VHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encapsulate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Hard Disk Drive (HDD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Aperture Cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Aperture Cards -- Acetate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floppy Disk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Aperture Cards -- Cellulose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Aperture Cards -- Nitrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Aperture Cards -- Silver Halide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network Attached Storage (NAS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfiche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfiche -- Acetate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHBX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfiche -- Cellulose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portable Universal Serial Bus (USB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfiche -- Nitrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfiche -- Silver Halide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOLBX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfilm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfilm -- Acetate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfilm -- Cellulose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfilm -- Nitrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform -- Microfilm -- Silver Halide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motion Picture Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motion Picture Film -- 16 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motion Picture Film -- 35 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motion Picture Film -- 70 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motion Picture Film -- 8 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motion Picture Film -- 9.5 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motion Picture Film -- Super 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Glass Plate Negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Lantern Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Mounted Slide Frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Mounted Slide Frame -- 110 Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Mounted Slide Frame -- 126 Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Mounted Slide Frame -- 127 Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Mounted Slide Frame -- 127 Super Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Mounted Slide Frame -- 35 mm Half Frame Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Mounted Slide Frame -- 35 mm Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative, Slide or Transparency -- Polyester Negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object -- Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object -- Metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object -- Plastic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object -- Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object -- Textile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object -- Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optical Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optical Media -- Compact Disc (CD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optical Media -- Digital Versatile Disc (DVD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper -- Blueprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper -- Cardboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper -- Mounted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper -- Synthetic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper -- Tracing / Offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phonographic Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phonographic Media -- Acetate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phonographic Media -- Shellac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phonographic Media -- Vinyl Disc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phonographic Media -- Wax Cylinder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Glass Plate Negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Transparency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic Print</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic Print -- Album</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic Print -- Framed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic Print -- Loose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic Print -- Mounted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic Print -- Sleeved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plastic Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vellum or Parchment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume -- Bolted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume -- Kalamazoo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume -- Locked</t>
   </si>
 </sst>
 </file>
@@ -123,7 +553,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -161,8 +591,46 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,7 +640,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF0F0F0"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF666666"/>
       </patternFill>
     </fill>
   </fills>
@@ -217,7 +691,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,6 +702,38 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -242,7 +748,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFF0F0F0"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -259,7 +765,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFF0F0F0"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -281,7 +787,7 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF4472C4"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
@@ -302,18 +808,82 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Boolean" displayName="Boolean" ref="B2:B4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name=""/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ContainedWithin" displayName="ContainedWithin" ref="E2:E37" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name=""/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="CopyrightStatus" displayName="CopyrightStatus" ref="H2:H4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name=""/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="DateQualifier" displayName="DateQualifier" ref="C2:C4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name=""/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Format" displayName="Format" ref="D2:D92" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name=""/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="RecordType" displayName="RecordType" ref="A2:A4" headerRowCount="0" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="ITM"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="SensitivityLabel" displayName="SensitivityLabel" ref="F2:F4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name=""/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Significance" displayName="Significance" ref="G2:G6" headerRowCount="0" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="Column1"/>
+  </tableColumns>
+</table>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T1048576"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -331,7 +901,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="18.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
@@ -461,10 +1031,49 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <dataValidations count="10">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E1002" type="list">
+      <formula1>INDIRECT("Format")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A2" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A3:A1002" type="list">
+      <formula1>INDIRECT("RecordType")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G3:G1002" type="list">
+      <formula1>INDIRECT("DateQualifier")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I3:I1002" type="list">
+      <formula1>INDIRECT("DateQualifier")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L3:L1002" type="list">
+      <formula1>INDIRECT("ContainedWithin")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M3:M1002" type="list">
+      <formula1>INDIRECT("SensitivityLabel")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P3:P1002" type="list">
+      <formula1>INDIRECT("Significance")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q3:Q1002" type="list">
+      <formula1>INDIRECT("Boolean")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R3:R1002" type="list">
+      <formula1>INDIRECT("CopyrightStatus")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -480,13 +1089,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1048576"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.82"/>
@@ -606,11 +1215,33 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:D1002" type="list">
+      <formula1>INDIRECT("Format")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F3:F1002" type="list">
+      <formula1>INDIRECT("DateQualifier")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H3:H1002" type="list">
+      <formula1>INDIRECT("DateQualifier")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K3:K1002" type="list">
+      <formula1>INDIRECT("ContainedWithin")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L3:L1002" type="list">
+      <formula1>INDIRECT("SensitivityLabel")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N3:N1002" type="list">
+      <formula1>INDIRECT("CopyrightStatus")</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -619,4 +1250,793 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H92"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="75.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="62.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="64.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="9" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D43" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D44" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D46" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D47" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D48" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D49" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D50" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D51" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D52" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D53" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D54" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D55" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D56" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D57" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D58" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D59" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D60" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D61" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D62" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D64" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D65" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D66" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D67" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D68" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D69" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D70" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D71" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D72" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D73" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D74" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D75" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D76" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D77" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D78" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D79" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D80" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D81" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D82" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D83" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D84" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D85" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D86" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D87" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D88" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D89" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D90" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D91" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D92" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Default to the create sheet
</commit_message>
<xml_diff>
--- a/bulk_edit_template.xlsx
+++ b/bulk_edit_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beth Battrick\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5395EF0-0C42-457E-BA91-0EE3FF29910E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0E258D-4913-4303-BFE4-48D0C64B613A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Records to Create" sheetId="1" r:id="rId1"/>
@@ -1257,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1613,7 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Updates for legacy processing sheet
  * Transfer ID is now required when creating a record

  * Dates can now support partial updates.  For example, you can
    change the certainty of an existing date without specifying the
    other date fields.
</commit_message>
<xml_diff>
--- a/bulk_edit_template.xlsx
+++ b/bulk_edit_template.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beth Battrick\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0E258D-4913-4303-BFE4-48D0C64B613A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CF1607-FADF-4EB3-B12F-F02533D75A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Records to Create" sheetId="1" r:id="rId1"/>
     <sheet name="Records to Update" sheetId="2" r:id="rId2"/>
     <sheet name="Vocabularies" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="247">
   <si>
     <t>Required</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Architectural or technical drawing</t>
   </si>
   <si>
-    <t>ALB</t>
-  </si>
-  <si>
     <t>This may contain information or photographs which some people may find distressing or offensive.</t>
   </si>
   <si>
@@ -167,12 +164,6 @@
     <t>exact</t>
   </si>
   <si>
-    <t>Chart (produced by machine)</t>
-  </si>
-  <si>
-    <t>ARCBX</t>
-  </si>
-  <si>
     <t>This may contain terms or images which Aboriginal and Torres Strait Islander people may find distressing or offensive.</t>
   </si>
   <si>
@@ -182,12 +173,6 @@
     <t>copyright_state_of_queensland</t>
   </si>
   <si>
-    <t>Drafting Cloth (Linen)</t>
-  </si>
-  <si>
-    <t>BUN</t>
-  </si>
-  <si>
     <t>memory_of_the_world</t>
   </si>
   <si>
@@ -200,365 +185,596 @@
     <t>standard</t>
   </si>
   <si>
-    <t>Magnetic Media</t>
-  </si>
-  <si>
-    <t>CBX</t>
-  </si>
-  <si>
-    <t>Magnetic Media -- Cartridge Tape</t>
-  </si>
-  <si>
-    <t>CDR</t>
-  </si>
-  <si>
-    <t>Magnetic Media -- Cassette Tape</t>
-  </si>
-  <si>
-    <t>Compact Disc (CD)</t>
-  </si>
-  <si>
-    <t>Magnetic Media -- Floppy Disk</t>
-  </si>
-  <si>
     <t>Core</t>
   </si>
   <si>
-    <t>Magnetic Media -- Hard Disc Drive</t>
-  </si>
-  <si>
-    <t>Digital Versatile Disc (DVD)</t>
-  </si>
-  <si>
-    <t>Magnetic Media -- Reel Tape</t>
-  </si>
-  <si>
-    <t>Digital media - Floppy disc - 3 1/2"</t>
-  </si>
-  <si>
-    <t>Magnetic Media -- Reel Tape -- 21 Track</t>
-  </si>
-  <si>
-    <t>Digital media - Floppy disc - 5 1/4"</t>
-  </si>
-  <si>
-    <t>Magnetic Media -- Reel Tape -- 7 Track</t>
-  </si>
-  <si>
-    <t>Digital media - Floppy disc - 8"</t>
-  </si>
-  <si>
-    <t>Magnetic Media -- Reel Tape -- 9 Track</t>
-  </si>
-  <si>
     <t>Digital media - LTO computer tape</t>
   </si>
   <si>
-    <t>Magnetic Media -- Video Tape</t>
-  </si>
-  <si>
-    <t>Digital media - Other</t>
-  </si>
-  <si>
-    <t>Magnetic Media -- Video Tape -- Betamax</t>
-  </si>
-  <si>
     <t>Digital media - PC</t>
   </si>
   <si>
-    <t>Magnetic Media -- Video Tape -- U-Matic</t>
-  </si>
-  <si>
     <t>Digital media - Server</t>
   </si>
   <si>
-    <t>Magnetic Media -- Video Tape -- VHS</t>
-  </si>
-  <si>
-    <t>Encapsulate</t>
-  </si>
-  <si>
-    <t>Microform</t>
-  </si>
-  <si>
-    <t>External Hard Disk Drive (HDD)</t>
-  </si>
-  <si>
-    <t>Microform -- Aperture Cards</t>
-  </si>
-  <si>
-    <t>FLM</t>
-  </si>
-  <si>
-    <t>Microform -- Aperture Cards -- Acetate</t>
-  </si>
-  <si>
-    <t>Floppy Disk</t>
-  </si>
-  <si>
-    <t>Microform -- Aperture Cards -- Cellulose</t>
-  </si>
-  <si>
-    <t>MBX</t>
-  </si>
-  <si>
-    <t>Microform -- Aperture Cards -- Nitrate</t>
-  </si>
-  <si>
-    <t>NAA</t>
-  </si>
-  <si>
-    <t>Microform -- Aperture Cards -- Silver Halide</t>
-  </si>
-  <si>
-    <t>Network Attached Storage (NAS)</t>
-  </si>
-  <si>
-    <t>Microform -- Microfiche</t>
-  </si>
-  <si>
-    <t>OTH</t>
-  </si>
-  <si>
-    <t>Microform -- Microfiche -- Acetate</t>
-  </si>
-  <si>
-    <t>PHBX</t>
-  </si>
-  <si>
-    <t>Microform -- Microfiche -- Cellulose</t>
-  </si>
-  <si>
-    <t>Portable Universal Serial Bus (USB)</t>
-  </si>
-  <si>
-    <t>Microform -- Microfiche -- Nitrate</t>
-  </si>
-  <si>
-    <t>SLD</t>
-  </si>
-  <si>
-    <t>Microform -- Microfiche -- Silver Halide</t>
-  </si>
-  <si>
-    <t>SOLBX</t>
-  </si>
-  <si>
-    <t>Microform -- Microfilm</t>
-  </si>
-  <si>
-    <t>TYPE1</t>
-  </si>
-  <si>
-    <t>Microform -- Microfilm -- Acetate</t>
-  </si>
-  <si>
-    <t>TYPE2</t>
-  </si>
-  <si>
-    <t>Microform -- Microfilm -- Cellulose</t>
-  </si>
-  <si>
-    <t>TYPE6</t>
-  </si>
-  <si>
-    <t>Microform -- Microfilm -- Nitrate</t>
-  </si>
-  <si>
-    <t>TYPE10</t>
-  </si>
-  <si>
-    <t>Microform -- Microfilm -- Silver Halide</t>
-  </si>
-  <si>
-    <t>TYPE11</t>
-  </si>
-  <si>
-    <t>Motion Picture Film</t>
-  </si>
-  <si>
-    <t>TYPE31</t>
-  </si>
-  <si>
-    <t>Motion Picture Film -- 16 mm</t>
-  </si>
-  <si>
-    <t>TYPE51</t>
-  </si>
-  <si>
-    <t>Motion Picture Film -- 35 mm</t>
-  </si>
-  <si>
-    <t>Motion Picture Film -- 70 mm</t>
-  </si>
-  <si>
-    <t>Motion Picture Film -- 8 mm</t>
-  </si>
-  <si>
-    <t>Motion Picture Film -- 9.5 mm</t>
-  </si>
-  <si>
-    <t>Motion Picture Film -- Super 8</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Glass Plate Negative</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Lantern Slide</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Mounted Slide Frame</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Mounted Slide Frame -- 110 Slide</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Mounted Slide Frame -- 126 Slide</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Mounted Slide Frame -- 127 Slide</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Mounted Slide Frame -- 127 Super Slide</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Mounted Slide Frame -- 35 mm Half Frame Slide</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Mounted Slide Frame -- 35 mm Slide</t>
-  </si>
-  <si>
-    <t>Negative, Slide or Transparency -- Polyester Negative</t>
-  </si>
-  <si>
-    <t>Not Set</t>
-  </si>
-  <si>
     <t>Object</t>
   </si>
   <si>
-    <t>Object -- Glass</t>
-  </si>
-  <si>
-    <t>Object -- Metal</t>
-  </si>
-  <si>
-    <t>Object -- Plastic</t>
-  </si>
-  <si>
-    <t>Object -- Stone</t>
-  </si>
-  <si>
-    <t>Object -- Textile</t>
-  </si>
-  <si>
-    <t>Object -- Wood</t>
-  </si>
-  <si>
-    <t>Optical Media</t>
-  </si>
-  <si>
-    <t>Optical Media -- Compact Disc (CD)</t>
-  </si>
-  <si>
-    <t>Optical Media -- Digital Versatile Disc (DVD)</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Paper</t>
-  </si>
-  <si>
-    <t>Paper -- Blueprint</t>
-  </si>
-  <si>
-    <t>Paper -- Cardboard</t>
-  </si>
-  <si>
-    <t>Paper -- Mounted</t>
-  </si>
-  <si>
-    <t>Paper -- Synthetic</t>
-  </si>
-  <si>
-    <t>Paper -- Tracing / Offset</t>
-  </si>
-  <si>
-    <t>Phonographic Media</t>
-  </si>
-  <si>
-    <t>Phonographic Media -- Acetate</t>
-  </si>
-  <si>
-    <t>Phonographic Media -- Shellac</t>
-  </si>
-  <si>
-    <t>Phonographic Media -- Vinyl Disc</t>
-  </si>
-  <si>
-    <t>Phonographic Media -- Wax Cylinder</t>
-  </si>
-  <si>
-    <t>Photographic - Glass Plate Negative</t>
-  </si>
-  <si>
-    <t>Photographic - Negative</t>
-  </si>
-  <si>
     <t>Photographic - Slide</t>
   </si>
   <si>
-    <t>Photographic - Transparency</t>
-  </si>
-  <si>
-    <t>Photographic Print</t>
-  </si>
-  <si>
-    <t>Photographic Print -- Album</t>
-  </si>
-  <si>
-    <t>Photographic Print -- Framed</t>
-  </si>
-  <si>
-    <t>Photographic Print -- Loose</t>
-  </si>
-  <si>
-    <t>Photographic Print -- Mounted</t>
-  </si>
-  <si>
-    <t>Photographic Print -- Sleeved</t>
-  </si>
-  <si>
-    <t>Plastic Film</t>
-  </si>
-  <si>
-    <t>Vellum or Parchment</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Volume -- Bolted</t>
-  </si>
-  <si>
-    <t>Volume -- Kalamazoo</t>
-  </si>
-  <si>
-    <t>Volume -- Locked</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Digital media - External hard drive</t>
+  </si>
+  <si>
+    <t>Digital media - Flashdrive/USB/Thumbdrive</t>
+  </si>
+  <si>
+    <t>Digital media - Floppy disk - 3 1/2"</t>
+  </si>
+  <si>
+    <t>Digital media - Floppy disk - 5 1/4"</t>
+  </si>
+  <si>
+    <t>Digital media - Floppy disk - 8"</t>
+  </si>
+  <si>
+    <t>Digital media - Internal hard drive</t>
+  </si>
+  <si>
+    <t>Digital media - Network Attached Storage (NAS)</t>
+  </si>
+  <si>
+    <t>Digital media - Optical  - CD</t>
+  </si>
+  <si>
+    <t>Digital media - Optical  - DVD</t>
+  </si>
+  <si>
+    <t>Digital Media - Other</t>
+  </si>
+  <si>
+    <t>Album</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Box - Card Box</t>
+  </si>
+  <si>
+    <t>Box - Microfilm Box</t>
+  </si>
+  <si>
+    <t>Box - Phase Box</t>
+  </si>
+  <si>
+    <t>Box - Solander Box</t>
+  </si>
+  <si>
+    <t>Box - Type 1</t>
+  </si>
+  <si>
+    <t>Box - Type 1 (Archival)</t>
+  </si>
+  <si>
+    <t>Box - Type 10</t>
+  </si>
+  <si>
+    <t>Box - Type 10 (Archival)</t>
+  </si>
+  <si>
+    <t>Box - Type 11</t>
+  </si>
+  <si>
+    <t>Box - Type 11 (Archival)</t>
+  </si>
+  <si>
+    <t>Box - Type 2</t>
+  </si>
+  <si>
+    <t>Box - Type 2 (Archival)</t>
+  </si>
+  <si>
+    <t>Box - Type 3</t>
+  </si>
+  <si>
+    <t>Box - Type 3 (Archival)</t>
+  </si>
+  <si>
+    <t>Box - Type 5</t>
+  </si>
+  <si>
+    <t>Box - Type 5 (Archival)</t>
+  </si>
+  <si>
+    <t>Box - Type 6</t>
+  </si>
+  <si>
+    <t>Box - Type 6 (Archival)</t>
+  </si>
+  <si>
+    <t>Bundle</t>
+  </si>
+  <si>
+    <t>Canister</t>
+  </si>
+  <si>
+    <t>Canister - Film - Aerial</t>
+  </si>
+  <si>
+    <t>Canister - Film - non-vented</t>
+  </si>
+  <si>
+    <t>Canister - Film - vented</t>
+  </si>
+  <si>
+    <t>Carousel - Slide Carousel</t>
+  </si>
+  <si>
+    <t>Drawer - Card Drawer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encapsulate </t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>Folder - Map</t>
+  </si>
+  <si>
+    <t>Hanger</t>
+  </si>
+  <si>
+    <t>No Container</t>
+  </si>
+  <si>
+    <t>Wrapping</t>
+  </si>
+  <si>
+    <t>Architectural or technical drawing - Blueprint - negative</t>
+  </si>
+  <si>
+    <t>Architectural or technical drawing - Blueprint - positive</t>
+  </si>
+  <si>
+    <t>Architectural or technical drawing - Composite</t>
+  </si>
+  <si>
+    <t>Architectural or technical drawing - Film</t>
+  </si>
+  <si>
+    <t>Architectural or technical drawing - Linen</t>
+  </si>
+  <si>
+    <t>Architectural or technical drawing - Paper</t>
+  </si>
+  <si>
+    <t>Artwork</t>
+  </si>
+  <si>
+    <t>Artwork - Banner</t>
+  </si>
+  <si>
+    <t>Artwork - Painting - framed</t>
+  </si>
+  <si>
+    <t>Artwork - Painting - unframed</t>
+  </si>
+  <si>
+    <t>Artwork - Poster - framed</t>
+  </si>
+  <si>
+    <t>Artwork - Poster - unframed</t>
+  </si>
+  <si>
+    <t>Artwork - Print - framed</t>
+  </si>
+  <si>
+    <t>Artwork - Print - unframed</t>
+  </si>
+  <si>
+    <t>Artwork - Sketch - framed</t>
+  </si>
+  <si>
+    <t>Artwork - Sketch - unframed</t>
+  </si>
+  <si>
+    <t>Cards</t>
+  </si>
+  <si>
+    <t>Cards - Punchcard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chart (produced by machine) </t>
+  </si>
+  <si>
+    <t>Chart (produced by machine) - Machine-generated (eg seismic, gyro)</t>
+  </si>
+  <si>
+    <t>Chart (produced by machine) - Stenotype Tape/Paper</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>File/document</t>
+  </si>
+  <si>
+    <t>File/document - Paper</t>
+  </si>
+  <si>
+    <t>File/document - Parchment</t>
+  </si>
+  <si>
+    <t>Film (roll) - Aerial film roll - acetate</t>
+  </si>
+  <si>
+    <t>Film (roll) - Aerial film roll - polyester</t>
+  </si>
+  <si>
+    <t>Film (roll) - Motion picture - 16mm - acetate</t>
+  </si>
+  <si>
+    <t>Film (roll) - Motion picture - 16mm - polyester</t>
+  </si>
+  <si>
+    <t>Film (roll) - Motion picture - 35mm - acetate</t>
+  </si>
+  <si>
+    <t>Film (roll) - Motion picture - 35mm - polyester</t>
+  </si>
+  <si>
+    <t>Film (roll) - Motion picture - 8mm - acetate</t>
+  </si>
+  <si>
+    <t>Film (roll) - Motion picture - 8mm - polyester</t>
+  </si>
+  <si>
+    <t>Film (roll) - Motion picture - Super 8 - acetate</t>
+  </si>
+  <si>
+    <t>Film (roll) - Motion picture - Super 8 - poylester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Film (video) </t>
+  </si>
+  <si>
+    <t>Film (video) - 1" tape</t>
+  </si>
+  <si>
+    <t>Film (video) - 2" tape</t>
+  </si>
+  <si>
+    <t>Film (video) - Betacam</t>
+  </si>
+  <si>
+    <t>Film (video) - Betamax</t>
+  </si>
+  <si>
+    <t>Film (video) - Super VHS</t>
+  </si>
+  <si>
+    <t>Film (video) - U-Matic 3/4"</t>
+  </si>
+  <si>
+    <t>Film (video) - U-Matic small</t>
+  </si>
+  <si>
+    <t>Film (video) - VHS</t>
+  </si>
+  <si>
+    <t>Film (video) - Video casette other (handicam)</t>
+  </si>
+  <si>
+    <t>Map/plan</t>
+  </si>
+  <si>
+    <t>Map/plan - Blueprint - negative</t>
+  </si>
+  <si>
+    <t>Map/plan - Blueprint - positive</t>
+  </si>
+  <si>
+    <t>Map/plan - Composite</t>
+  </si>
+  <si>
+    <t>Map/plan - Film</t>
+  </si>
+  <si>
+    <t>Map/plan - Linen</t>
+  </si>
+  <si>
+    <t>Map/plan - Paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform </t>
+  </si>
+  <si>
+    <t>Microform - Aperture card</t>
+  </si>
+  <si>
+    <t>Microform - Microfiche</t>
+  </si>
+  <si>
+    <t>Microform - Microfilm</t>
+  </si>
+  <si>
+    <t>Microform - Microfilm - 16mm - Duplicate</t>
+  </si>
+  <si>
+    <t>Microform - Microfilm - 16mm - Master</t>
+  </si>
+  <si>
+    <t>Microform - Microfilm - 16mm - Security</t>
+  </si>
+  <si>
+    <t>Microform - Microfilm - 35mm - Duplicate</t>
+  </si>
+  <si>
+    <t>Microform - Microfilm - 35mm - Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microform - Microfilm - 35mm - Security </t>
+  </si>
+  <si>
+    <t>Microform - Microfilm - Duplicate</t>
+  </si>
+  <si>
+    <t>Microform - Microfilm - Master</t>
+  </si>
+  <si>
+    <t>Microform - Microfilm - Security</t>
+  </si>
+  <si>
+    <t>Object - Architectural model/marquette</t>
+  </si>
+  <si>
+    <t>Object - Currency</t>
+  </si>
+  <si>
+    <t>Object - Honour Board</t>
+  </si>
+  <si>
+    <t>Object - Medals</t>
+  </si>
+  <si>
+    <t>Object - Printing Blocks</t>
+  </si>
+  <si>
+    <t>Object - Specimens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic </t>
+  </si>
+  <si>
+    <t>Tape - sound recording</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume/register </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume/register - Album </t>
+  </si>
+  <si>
+    <t>Volume/register - Copy Press (iron gall ink)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume/register - Copy Press (letterpress) </t>
+  </si>
+  <si>
+    <t>Volume/register - Notebook</t>
+  </si>
+  <si>
+    <t>Volume/register - Parchment</t>
+  </si>
+  <si>
+    <t>Volume/register - Perfect bound</t>
+  </si>
+  <si>
+    <t>Volume/register - Post bound</t>
+  </si>
+  <si>
+    <t>Volume/register - Register - leather bound</t>
+  </si>
+  <si>
+    <t>Volume/register - Register - non leather bound</t>
+  </si>
+  <si>
+    <t>Volume/register - Ring bound</t>
+  </si>
+  <si>
+    <t>Volume/register - Spiral bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Glass Plate Negative </t>
+  </si>
+  <si>
+    <t>Photographic - Glass Plate Negative - full plate</t>
+  </si>
+  <si>
+    <t>Photographic - Glass Plate Negative - half plate</t>
+  </si>
+  <si>
+    <t>Photographic - Glass Plate Negative - lantern slide</t>
+  </si>
+  <si>
+    <t>Photographic - Glass Plate Negative - mammoth</t>
+  </si>
+  <si>
+    <t>Photographic - Glass Plate Negative - quarter plate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Negative </t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 120 - B&amp;W - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 120 - B&amp;W - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 120 - B&amp;W - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 120 - Colour - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 120 - Colour - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 120 - Colour - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 35mm - B&amp;W - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 35mm - B&amp;W - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 35mm - B&amp;W - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 35mm - Colour - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 35mm - Colour - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 35mm - Colour - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 4 x 5 - B&amp;W - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 4 x 5 - B&amp;W - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 4 x 5 - B&amp;W - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 8 x 10 - B&amp;W - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 8 x 10 - B&amp;W - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Negative - 8 x 10 - B&amp;W - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Print</t>
+  </si>
+  <si>
+    <t>Photographic - Print - B&amp;W</t>
+  </si>
+  <si>
+    <t>Photographic - Print - Colour</t>
+  </si>
+  <si>
+    <t>Photographic - Print - framed</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 120 - B&amp;W - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 120 - B&amp;W - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 120 - B&amp;W - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 120 - Colour - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 120 - Colour - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 120 - Colour - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 35mm - B&amp;W - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 35mm - B&amp;W - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 35mm - B&amp;W - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 35mm - Colour - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 35mm - Colour - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Slide - 35mm - Colour - undetermined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Transparency </t>
+  </si>
+  <si>
+    <t>Photographic - Transparency 120 - colour - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Transparency 120 - colour - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Transparency 120 - colour - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Transparency 35mm - colour - acetate</t>
+  </si>
+  <si>
+    <t>Photographic - Transparency 35mm - colour - polyester</t>
+  </si>
+  <si>
+    <t>Photographic - Transparency 35mm - colour - undetermined</t>
+  </si>
+  <si>
+    <t>Photographic - Transparency 4 x 5 - colour</t>
+  </si>
+  <si>
+    <t>Photographic - Print - Aerial</t>
+  </si>
+  <si>
+    <t>Photographic - Print - Aerial - B&amp;W</t>
+  </si>
+  <si>
+    <t>Photographic - Print - Aerial - colour</t>
+  </si>
+  <si>
+    <t>Tape - sound recording - 8 Track audio</t>
+  </si>
+  <si>
+    <t>Tape - sound recording - Audio 1" reel</t>
+  </si>
+  <si>
+    <t>Tape - sound recording - Audio 1/4" reel</t>
+  </si>
+  <si>
+    <t>Tape - sound recording - Audio 2" reel</t>
+  </si>
+  <si>
+    <t>Tape - sound recording - Compact casette</t>
+  </si>
+  <si>
+    <t>Tape - sound recording - Micro cassette</t>
+  </si>
+  <si>
+    <t>Tape - sound recording - Mini cassette</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -607,6 +823,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -649,7 +878,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -659,9 +888,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -680,11 +906,103 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -887,7 +1205,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Boolean" displayName="Boolean" ref="B2:B4" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Boolean" displayName="Boolean" ref="B2:B4" totalsRowShown="0" headerRowDxfId="9">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name=" "/>
   </tableColumns>
@@ -896,16 +1214,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ContainedWithin" displayName="ContainedWithin" ref="E2:E37" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ContainedWithin" displayName="ContainedWithin" ref="E2:E51" totalsRowShown="0" headerRowDxfId="8" dataDxfId="2">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name=" "/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name=" " dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="DateQualifier" displayName="DateQualifier" ref="C2:C4" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="DateQualifier" displayName="DateQualifier" ref="C2:C4" totalsRowShown="0" headerRowDxfId="7">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name=" "/>
   </tableColumns>
@@ -914,9 +1232,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Format" displayName="Format" ref="D2:D92" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Format" displayName="Format" ref="D2:D151" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name=" "/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name=" " dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -932,7 +1250,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="SensitivityLabel" displayName="SensitivityLabel" ref="F2:F4" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="SensitivityLabel" displayName="SensitivityLabel" ref="F2:F4" totalsRowShown="0" headerRowDxfId="5">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name=" "/>
   </tableColumns>
@@ -950,7 +1268,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="CopyrightStatus" displayName="CopyrightStatus" ref="H2:H4" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="CopyrightStatus" displayName="CopyrightStatus" ref="H2:H4" totalsRowShown="0" headerRowDxfId="4">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name=" "/>
   </tableColumns>
@@ -1257,35 +1575,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.1328125" customWidth="1"/>
+    <col min="3" max="3" width="9.265625" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" customWidth="1"/>
+    <col min="6" max="6" width="40.73046875" customWidth="1"/>
+    <col min="7" max="7" width="19.1328125" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.265625" customWidth="1"/>
+    <col min="10" max="10" width="23.59765625" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.3984375" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" customWidth="1"/>
-    <col min="17" max="17" width="33.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.59765625" customWidth="1"/>
+    <col min="15" max="15" width="19.59765625" customWidth="1"/>
+    <col min="16" max="16" width="12.86328125" customWidth="1"/>
+    <col min="17" max="17" width="33.59765625" customWidth="1"/>
     <col min="18" max="19" width="18" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" customWidth="1"/>
-    <col min="21" max="1025" width="11.5703125"/>
+    <col min="20" max="20" width="9.73046875" customWidth="1"/>
+    <col min="21" max="1025" width="11.59765625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1347,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1410,8 +1728,8 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E3:E1002" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="11">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E4:E1002" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT("Format")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1427,7 +1745,7 @@
       <formula1>INDIRECT("DateQualifier")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="L3:L1002" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="L4:L1002" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>INDIRECT("ContainedWithin")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1447,6 +1765,12 @@
       <formula1>INDIRECT("CopyrightStatus")</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E3" xr:uid="{2B736061-D5E6-4DF4-8CD8-0E6B7162EBBA}">
+      <formula1>INDIRECT("Format")</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="L3" xr:uid="{757C2F83-5568-47CF-A261-4F464D7435B4}">
+      <formula1>INDIRECT("ContainedWithin")</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1457,31 +1781,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.1328125" customWidth="1"/>
+    <col min="2" max="2" width="38.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" customWidth="1"/>
+    <col min="4" max="4" width="20.73046875" customWidth="1"/>
+    <col min="5" max="5" width="40.73046875" customWidth="1"/>
+    <col min="6" max="6" width="19.1328125" customWidth="1"/>
     <col min="7" max="7" width="40" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.265625" customWidth="1"/>
+    <col min="9" max="9" width="23.59765625" customWidth="1"/>
+    <col min="10" max="10" width="17.3984375" customWidth="1"/>
+    <col min="11" max="11" width="20.73046875" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.59765625" customWidth="1"/>
     <col min="14" max="15" width="18" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" customWidth="1"/>
-    <col min="17" max="1025" width="11.5703125"/>
+    <col min="16" max="16" width="9.73046875" customWidth="1"/>
+    <col min="17" max="1025" width="11.59765625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -1582,8 +1906,8 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D3:D1002" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="7">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D4:D1002" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>INDIRECT("Format")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1591,7 +1915,7 @@
       <formula1>INDIRECT("DateQualifier")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="K3:K1002" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="K4:K1002" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>INDIRECT("ContainedWithin")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1603,6 +1927,12 @@
       <formula1>INDIRECT("CopyrightStatus")</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="K3" xr:uid="{2C1C3815-0903-4DA2-8C3B-1F5ECA756F22}">
+      <formula1>INDIRECT("ContainedWithin")</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D3" xr:uid="{90A45981-9B1E-4027-90A4-F994450BA21F}">
+      <formula1>INDIRECT("Format")</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1611,76 +1941,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="75.85546875" customWidth="1"/>
-    <col min="5" max="5" width="62.85546875" customWidth="1"/>
+    <col min="1" max="2" width="17.3984375" customWidth="1"/>
+    <col min="3" max="3" width="15.86328125" customWidth="1"/>
+    <col min="4" max="4" width="75.86328125" customWidth="1"/>
+    <col min="5" max="5" width="62.86328125" customWidth="1"/>
     <col min="6" max="6" width="64" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
-    <col min="9" max="1023" width="8.85546875" customWidth="1"/>
-    <col min="1024" max="1025" width="11.5703125"/>
+    <col min="7" max="7" width="21.86328125" customWidth="1"/>
+    <col min="8" max="8" width="26.59765625" customWidth="1"/>
+    <col min="9" max="1023" width="8.86328125" customWidth="1"/>
+    <col min="1024" max="1025" width="11.59765625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1690,700 +2022,1034 @@
       <c r="C3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" t="s">
         <v>40</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>52</v>
+      <c r="D5" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>55</v>
+      <c r="D6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>58</v>
+      <c r="D7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>60</v>
+      <c r="D8" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>62</v>
+      <c r="D9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>64</v>
+      <c r="D10" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>66</v>
+      <c r="D11" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>68</v>
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" t="s">
+      <c r="D13" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>72</v>
+      <c r="D14" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>74</v>
+      <c r="D15" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>76</v>
+      <c r="D16" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>78</v>
+      <c r="D17" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>80</v>
+      <c r="D18" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>82</v>
+      <c r="D19" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>84</v>
+      <c r="D20" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>86</v>
+      <c r="D21" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>88</v>
+      <c r="D22" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>90</v>
+      <c r="D23" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>92</v>
+      <c r="D24" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>94</v>
+      <c r="D25" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>96</v>
+      <c r="D26" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>98</v>
+      <c r="D27" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>100</v>
+      <c r="D28" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>102</v>
+      <c r="D29" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>104</v>
+      <c r="D30" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>106</v>
+      <c r="D31" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>84</v>
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>108</v>
+      <c r="D32" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>110</v>
+      <c r="D33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>112</v>
+      <c r="D34" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>114</v>
+      <c r="D35" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>116</v>
+      <c r="D36" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>118</v>
+      <c r="D37" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" s="3"/>
+      <c r="D38" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E39" s="3"/>
+      <c r="D39" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D40" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E40" s="3"/>
+    <row r="40" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D40" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D43" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D45" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D47" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D48" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D50" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D51" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D52" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D53" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D54" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D55" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D57" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D58" t="s">
+    <row r="41" spans="2:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="D41" s="15" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D59" t="s">
+      <c r="E41" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D42" s="15" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
+      <c r="E42" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D43" s="15" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D61" t="s">
+      <c r="E43" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D44" s="15" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D62" t="s">
+      <c r="E44" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D45" s="15" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D63" t="s">
+      <c r="E45" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D46" s="15" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D64" t="s">
+      <c r="E46" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D47" s="15" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D65" t="s">
+      <c r="E47" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D48" s="15" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D66" t="s">
+      <c r="E48" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D49" s="15" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D67" t="s">
+      <c r="E49" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D50" s="14" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D68" t="s">
+      <c r="E50" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D51" s="14" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D69" t="s">
+      <c r="E51" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D52" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D70" t="s">
+    <row r="53" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D53" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D71" t="s">
+    <row r="54" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D54" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D72" t="s">
+    <row r="55" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D55" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D73" t="s">
+    <row r="56" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D56" s="14" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D74" t="s">
+    <row r="57" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D57" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D75" t="s">
+    <row r="58" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D58" s="15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D76" t="s">
+    <row r="59" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D59" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D77" t="s">
+    <row r="60" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D60" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D78" t="s">
+    <row r="61" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D61" s="15" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D79" t="s">
+    <row r="62" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D62" s="15" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D80" t="s">
+    <row r="63" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D63" s="15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D81" t="s">
+    <row r="64" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D64" s="15" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D82" t="s">
+    <row r="65" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D65" s="15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D83" t="s">
+    <row r="66" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D66" s="15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D84" t="s">
+    <row r="67" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D67" s="15" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D85" t="s">
+    <row r="68" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D68" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D86" t="s">
+    <row r="69" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D69" s="15" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D87" t="s">
+    <row r="70" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D70" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D71" s="15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D88" t="s">
+    <row r="72" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D72" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D89" t="s">
+    <row r="73" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D73" s="15" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D90" t="s">
+    <row r="74" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D74" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D91" t="s">
+    <row r="75" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D75" s="15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D92" t="s">
+    <row r="76" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D76" s="15" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D77" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D78" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D79" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D80" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D81" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D82" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D83" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D84" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D85" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D86" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D87" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D88" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D89" s="15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D90" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D91" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D92" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D93" s="15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="94" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D94" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D95" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="96" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D96" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D97" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D98" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D99" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D100" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D101" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D102" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D103" s="15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D104" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D105" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D106" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D107" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D108" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="109" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D109" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D110" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D111" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D112" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D113" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D114" s="15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D115" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="116" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D116" s="15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D117" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D118" s="15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="119" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D119" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D120" s="15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="121" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D121" s="15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="122" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D122" s="15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D123" s="15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="124" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D124" s="15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D125" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="126" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D126" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="127" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D127" s="15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="128" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D128" s="15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D129" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D130" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D131" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D132" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D133" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D134" s="15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D135" s="15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D136" s="15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D137" s="15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D138" s="15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D139" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D140" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D141" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D142" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D143" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D144" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D145" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D146" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D147" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="148" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D148" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D149" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D150" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
+      <c r="D151" s="14" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add latest version of bulk edit template
</commit_message>
<xml_diff>
--- a/bulk_edit_template.xlsx
+++ b/bulk_edit_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CF1607-FADF-4EB3-B12F-F02533D75A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C963DF-895B-4937-AE3D-36F23A4111CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Records to Create" sheetId="1" r:id="rId1"/>
@@ -236,9 +236,6 @@
     <t>Digital media - Optical  - DVD</t>
   </si>
   <si>
-    <t>Digital Media - Other</t>
-  </si>
-  <si>
     <t>Album</t>
   </si>
   <si>
@@ -768,6 +765,9 @@
   </si>
   <si>
     <t>Tape - sound recording - Mini cassette</t>
+  </si>
+  <si>
+    <t>Digital media - Other</t>
   </si>
 </sst>
 </file>
@@ -878,7 +878,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -922,6 +922,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,11 +945,32 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -981,45 +1009,6 @@
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1074,14 +1063,32 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
+        <sz val="10"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
+        <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1214,16 +1221,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ContainedWithin" displayName="ContainedWithin" ref="E2:E51" totalsRowShown="0" headerRowDxfId="8" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ContainedWithin" displayName="ContainedWithin" ref="E2:E51" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name=" " dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name=" " dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="DateQualifier" displayName="DateQualifier" ref="C2:C4" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="DateQualifier" displayName="DateQualifier" ref="C2:C4" totalsRowShown="0" headerRowDxfId="5">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name=" "/>
   </tableColumns>
@@ -1232,9 +1239,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Format" displayName="Format" ref="D2:D151" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Format" displayName="Format" ref="D2:D151" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name=" " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name=" " dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1250,7 +1257,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="SensitivityLabel" displayName="SensitivityLabel" ref="F2:F4" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="SensitivityLabel" displayName="SensitivityLabel" ref="F2:F4" totalsRowShown="0" headerRowDxfId="1">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name=" "/>
   </tableColumns>
@@ -1268,7 +1275,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="CopyrightStatus" displayName="CopyrightStatus" ref="H2:H4" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="CopyrightStatus" displayName="CopyrightStatus" ref="H2:H4" totalsRowShown="0" headerRowDxfId="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name=" "/>
   </tableColumns>
@@ -1586,11 +1593,11 @@
     <col min="3" max="3" width="9.265625" customWidth="1"/>
     <col min="4" max="4" width="12.1328125" customWidth="1"/>
     <col min="5" max="5" width="21.3984375" customWidth="1"/>
-    <col min="6" max="6" width="40.73046875" customWidth="1"/>
+    <col min="6" max="6" width="40.73046875" style="19" customWidth="1"/>
     <col min="7" max="7" width="19.1328125" customWidth="1"/>
-    <col min="8" max="8" width="40" customWidth="1"/>
+    <col min="8" max="8" width="40" style="19" customWidth="1"/>
     <col min="9" max="9" width="18.265625" customWidth="1"/>
-    <col min="10" max="10" width="23.59765625" customWidth="1"/>
+    <col min="10" max="10" width="23.59765625" style="19" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="21.3984375" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
@@ -1619,19 +1626,19 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="17" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1681,19 +1688,19 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="18" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="18" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="18" t="s">
         <v>16</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -1773,7 +1780,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1781,9 +1788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1791,11 +1796,11 @@
     <col min="2" max="2" width="38.86328125" customWidth="1"/>
     <col min="3" max="3" width="12.1328125" customWidth="1"/>
     <col min="4" max="4" width="20.73046875" customWidth="1"/>
-    <col min="5" max="5" width="40.73046875" customWidth="1"/>
+    <col min="5" max="5" width="40.73046875" style="19" customWidth="1"/>
     <col min="6" max="6" width="19.1328125" customWidth="1"/>
-    <col min="7" max="7" width="40" customWidth="1"/>
+    <col min="7" max="7" width="40" style="19" customWidth="1"/>
     <col min="8" max="8" width="18.265625" customWidth="1"/>
-    <col min="9" max="9" width="23.59765625" customWidth="1"/>
+    <col min="9" max="9" width="23.59765625" style="19" customWidth="1"/>
     <col min="10" max="10" width="17.3984375" customWidth="1"/>
     <col min="11" max="11" width="20.73046875" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
@@ -1818,19 +1823,19 @@
       <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1868,19 +1873,19 @@
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="18" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -1944,7 +1949,7 @@
   <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2049,7 +2054,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>61</v>
@@ -2068,7 +2073,7 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>62</v>
@@ -2082,7 +2087,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>63</v>
@@ -2096,7 +2101,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>64</v>
@@ -2107,7 +2112,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>65</v>
@@ -2118,7 +2123,7 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>53</v>
@@ -2129,7 +2134,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>66</v>
@@ -2140,7 +2145,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>67</v>
@@ -2151,7 +2156,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>68</v>
@@ -2162,10 +2167,10 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>69</v>
+        <v>246</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -2173,7 +2178,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>54</v>
@@ -2184,7 +2189,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>55</v>
@@ -2195,10 +2200,10 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -2206,10 +2211,10 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -2217,10 +2222,10 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -2228,7 +2233,7 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>50</v>
@@ -2239,10 +2244,10 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -2250,10 +2255,10 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -2261,10 +2266,10 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -2272,10 +2277,10 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -2283,10 +2288,10 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -2294,10 +2299,10 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="3"/>
     </row>
@@ -2305,10 +2310,10 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -2316,10 +2321,10 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -2327,10 +2332,10 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F28" s="3"/>
     </row>
@@ -2341,7 +2346,7 @@
         <v>49</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F29" s="3"/>
     </row>
@@ -2349,10 +2354,10 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" s="3"/>
     </row>
@@ -2360,10 +2365,10 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -2371,10 +2376,10 @@
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -2382,10 +2387,10 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -2393,10 +2398,10 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -2404,10 +2409,10 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -2415,10 +2420,10 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -2426,10 +2431,10 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -2437,10 +2442,10 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38" s="3"/>
     </row>
@@ -2448,41 +2453,41 @@
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D40" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="2:6" ht="13.15" x14ac:dyDescent="0.4">
       <c r="D41" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D42" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D43" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>52</v>
@@ -2490,55 +2495,55 @@
     </row>
     <row r="44" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D44" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D45" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D46" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D47" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D48" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D49" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D50" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>57</v>
@@ -2546,100 +2551,100 @@
     </row>
     <row r="51" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D51" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D52" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D53" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D54" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D55" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D56" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D57" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D58" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D59" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D60" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D61" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D62" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D63" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="4:5" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D64" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D65" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D66" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D67" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D68" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D69" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
@@ -2649,32 +2654,32 @@
     </row>
     <row r="71" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D71" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D72" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D73" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D74" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="75" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D75" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D76" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="77" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
@@ -2684,152 +2689,152 @@
     </row>
     <row r="78" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D78" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D79" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D80" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="81" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D81" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D82" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D83" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D84" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="85" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D85" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="86" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D86" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D87" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="88" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D88" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="89" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D89" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D90" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="91" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D91" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="92" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D92" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D93" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D94" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="95" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D95" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D96" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D97" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D98" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="99" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D99" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="100" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D100" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D101" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="102" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D102" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D103" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="104" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D104" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="105" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D105" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="106" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D106" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D107" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="108" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
@@ -2839,217 +2844,217 @@
     </row>
     <row r="109" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D109" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D110" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="111" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D111" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D112" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D113" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="114" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D114" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="115" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D115" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D116" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D117" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="118" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D118" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="119" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D119" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D120" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="121" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D121" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="122" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D122" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="123" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D123" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="124" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D124" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="125" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D125" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="126" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D126" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="127" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D127" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="128" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D128" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="129" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D129" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="130" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D130" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="131" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D131" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="132" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D132" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="133" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D133" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="134" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D134" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="135" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D135" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="136" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D136" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="137" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D137" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="138" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D138" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="139" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D139" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="140" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D140" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="141" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D141" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="142" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D142" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="143" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D143" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="144" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D144" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="145" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D145" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="146" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D146" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="147" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D147" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="148" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D148" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="149" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D149" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="150" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D150" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="151" spans="4:4" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D151" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Piv#171990568 update bulk_edit_template.xlsx with Transfer required label change
</commit_message>
<xml_diff>
--- a/bulk_edit_template.xlsx
+++ b/bulk_edit_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C963DF-895B-4937-AE3D-36F23A4111CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2315886D-7E98-4713-8F67-DC89429F8414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Records to Create" sheetId="1" r:id="rId1"/>
@@ -1582,9 +1582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1651,7 +1649,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>1</v>

</xml_diff>